<commit_message>
Charm Finder / Youtube Vid Instructions / Fix Stat ID for Hierophant Mana Reservation Efficiency
</commit_message>
<xml_diff>
--- a/html/charm-finder/charm-mods.xlsx
+++ b/html/charm-finder/charm-mods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Synology\Drive\GitHub\JustExileThings\html\charm-finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E223DC44-5AAF-4BA6-8D94-385853A9652C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F3EEC6-7AE3-45FE-9775-09BFFD8F9794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="30" windowWidth="38520" windowHeight="12030" xr2:uid="{14DC885A-69EC-4E76-AB19-C1EAD6A80126}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{14DC885A-69EC-4E76-AB19-C1EAD6A80126}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1690,14 +1690,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1305CC71-141C-484E-819D-D7798C70F2A4}">
   <dimension ref="A1:L243"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B232" sqref="B232"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.42578125" bestFit="1" customWidth="1"/>
@@ -5846,7 +5846,7 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>1212083058</v>
+        <v>4237190083</v>
       </c>
       <c r="B142" t="s">
         <v>29</v>
@@ -5878,7 +5878,7 @@
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>1212083058</v>
+        <v>4237190083</v>
       </c>
       <c r="B143" t="s">
         <v>29</v>

</xml_diff>